<commit_message>
Check whether everything works with a new field
</commit_message>
<xml_diff>
--- a/e2e/input_20240428.xlsx
+++ b/e2e/input_20240428.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\_Privat\webcon_playwright\e2e\automatedUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\_Privat\webcon_playwright\e2e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA3ACA4-AF7C-4285-BB4D-89190FC91C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF1BFAA-E76A-4D0D-8DA5-F08BB7D79A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FieldInformation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -516,7 +516,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D6:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
@@ -655,14 +655,14 @@
       <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>38</v>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
@@ -682,13 +682,15 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="3">
         <v>2</v>
       </c>
@@ -707,14 +709,14 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
@@ -734,14 +736,14 @@
       <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>38</v>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
@@ -766,8 +768,8 @@
       <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>38</v>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>

</xml_diff>